<commit_message>
added data from June 28 PW
</commit_message>
<xml_diff>
--- a/data/inventory/tags_PointWhitney_20240619.xlsx
+++ b/data/inventory/tags_PointWhitney_20240619.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/project-gigas-conditioning/data/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483E2FAA-D49C-2045-AB8C-669FD35400D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F226AD0A-045D-2C4B-BC58-E2E1FF596E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20680" yWindow="-1460" windowWidth="16700" windowHeight="18440" xr2:uid="{67E9221A-8E6D-0647-AD63-EB30BB1B3412}"/>
+    <workbookView xWindow="2020" yWindow="760" windowWidth="25800" windowHeight="17700" xr2:uid="{67E9221A-8E6D-0647-AD63-EB30BB1B3412}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="97">
   <si>
     <t>effort</t>
   </si>
@@ -252,6 +252,81 @@
   </si>
   <si>
     <t>LCO Spat Control 2</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>Triploid Control</t>
+  </si>
+  <si>
+    <t>2 week temperature Triploid</t>
+  </si>
+  <si>
+    <t>Triploid Treated</t>
+  </si>
+  <si>
+    <t>2 week temperature Diploid</t>
+  </si>
+  <si>
+    <t>Diploid Control</t>
+  </si>
+  <si>
+    <t>Diploid Treatment</t>
+  </si>
+  <si>
+    <t>PW Bulk Seed</t>
+  </si>
+  <si>
+    <t>2 week stressors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PW Seed </t>
+  </si>
+  <si>
+    <t>PW</t>
+  </si>
+  <si>
+    <t>UW-SR26</t>
+  </si>
+  <si>
+    <t>Dock lagoon; Point Whitney</t>
+  </si>
+  <si>
+    <t>UW-SR6</t>
+  </si>
+  <si>
+    <t>UW-SR27</t>
+  </si>
+  <si>
+    <t>UW-SR30</t>
+  </si>
+  <si>
+    <t>Immune</t>
+  </si>
+  <si>
+    <t>UW-SR23</t>
+  </si>
+  <si>
+    <t>Treated 35C</t>
+  </si>
+  <si>
+    <t>UW-SR14</t>
+  </si>
+  <si>
+    <t>UW-SR18</t>
+  </si>
+  <si>
+    <t>Treated FW35C</t>
+  </si>
+  <si>
+    <t>Treated FW</t>
+  </si>
+  <si>
+    <t>UW-SR5</t>
+  </si>
+  <si>
+    <t>UW-SR21</t>
   </si>
 </sst>
 </file>
@@ -647,10 +722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DE0C57-F120-E045-8B06-81048685F26B}">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,25 +773,25 @@
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -732,7 +808,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -758,25 +834,25 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
@@ -784,25 +860,25 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
@@ -810,25 +886,25 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
         <v>18</v>
@@ -836,25 +912,25 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
         <v>18</v>
@@ -862,25 +938,25 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
@@ -888,33 +964,33 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -926,47 +1002,47 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -978,21 +1054,21 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -1004,39 +1080,39 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="H14" t="s">
         <v>18</v>
@@ -1044,25 +1120,25 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="H15" t="s">
         <v>18</v>
@@ -1070,25 +1146,25 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
       </c>
       <c r="H16" t="s">
         <v>18</v>
@@ -1096,25 +1172,25 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>59</v>
       </c>
       <c r="H17" t="s">
         <v>18</v>
@@ -1122,13 +1198,13 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
@@ -1140,7 +1216,7 @@
         <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H18" t="s">
         <v>18</v>
@@ -1148,13 +1224,13 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
@@ -1166,7 +1242,7 @@
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
@@ -1174,16 +1250,16 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
@@ -1192,7 +1268,7 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H20" t="s">
         <v>18</v>
@@ -1200,25 +1276,25 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="H21" t="s">
         <v>18</v>
@@ -1226,10 +1302,10 @@
     </row>
     <row r="22" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
@@ -1238,13 +1314,13 @@
         <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
         <v>18</v>
@@ -1261,25 +1337,25 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="H23" t="s">
         <v>18</v>
@@ -1287,10 +1363,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
@@ -1299,13 +1375,13 @@
         <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="H24" t="s">
         <v>18</v>
@@ -1313,16 +1389,16 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E25" t="s">
         <v>30</v>
@@ -1331,7 +1407,7 @@
         <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H25" t="s">
         <v>18</v>
@@ -1339,16 +1415,16 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
         <v>30</v>
@@ -1357,7 +1433,7 @@
         <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H26" t="s">
         <v>18</v>
@@ -1365,16 +1441,16 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
         <v>30</v>
@@ -1383,7 +1459,7 @@
         <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H27" t="s">
         <v>18</v>
@@ -1391,25 +1467,25 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" t="s">
-        <v>54</v>
+        <v>15</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="H28" t="s">
         <v>18</v>
@@ -1417,25 +1493,25 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" t="s">
-        <v>55</v>
+        <v>15</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="H29" t="s">
         <v>18</v>
@@ -1443,51 +1519,51 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="H30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" t="s">
-        <v>50</v>
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>27.039000000000001</v>
       </c>
       <c r="F31" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" t="s">
-        <v>57</v>
+        <v>15</v>
+      </c>
+      <c r="G31">
+        <v>27.039000000000001</v>
       </c>
       <c r="H31" t="s">
         <v>18</v>
@@ -1495,28 +1571,28 @@
     </row>
     <row r="32" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="F32" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="H32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
@@ -1530,25 +1606,25 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" t="s">
-        <v>51</v>
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>27.024999999999999</v>
       </c>
       <c r="F33" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" t="s">
-        <v>61</v>
+        <v>15</v>
+      </c>
+      <c r="G33">
+        <v>27.024999999999999</v>
       </c>
       <c r="H33" t="s">
         <v>18</v>
@@ -1556,25 +1632,25 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
         <v>25</v>
       </c>
-      <c r="E34" t="s">
-        <v>52</v>
+      <c r="E34">
+        <v>27.052</v>
       </c>
       <c r="F34" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" t="s">
-        <v>59</v>
+        <v>15</v>
+      </c>
+      <c r="G34">
+        <v>27.052</v>
       </c>
       <c r="H34" t="s">
         <v>18</v>
@@ -1582,25 +1658,25 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
         <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="H35" t="s">
         <v>18</v>
@@ -1608,28 +1684,28 @@
     </row>
     <row r="36" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="F36" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="H36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I36"/>
       <c r="J36"/>
@@ -1643,28 +1719,28 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="F37" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="H37" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -1695,7 +1771,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>64</v>
@@ -1704,16 +1780,16 @@
         <v>65</v>
       </c>
       <c r="D39" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E39">
-        <v>27.024999999999999</v>
+        <v>27.009</v>
       </c>
       <c r="F39" t="s">
         <v>15</v>
       </c>
       <c r="G39">
-        <v>27.024999999999999</v>
+        <v>27.009</v>
       </c>
       <c r="H39" t="s">
         <v>18</v>
@@ -1721,25 +1797,25 @@
     </row>
     <row r="40" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="D40" t="s">
         <v>25</v>
       </c>
-      <c r="E40">
-        <v>27.052</v>
+      <c r="E40" t="s">
+        <v>30</v>
       </c>
       <c r="F40" t="s">
         <v>15</v>
       </c>
-      <c r="G40">
-        <v>27.052</v>
+      <c r="G40" t="s">
+        <v>39</v>
       </c>
       <c r="H40" t="s">
         <v>18</v>
@@ -1756,25 +1832,25 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
         <v>35</v>
       </c>
-      <c r="B41" t="s">
-        <v>64</v>
-      </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="D41" t="s">
         <v>25</v>
       </c>
-      <c r="E41">
-        <v>27.009</v>
+      <c r="E41" t="s">
+        <v>30</v>
       </c>
       <c r="F41" t="s">
         <v>15</v>
       </c>
-      <c r="G41">
-        <v>27.009</v>
+      <c r="G41" t="s">
+        <v>38</v>
       </c>
       <c r="H41" t="s">
         <v>18</v>
@@ -1782,28 +1858,28 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="D42" t="s">
         <v>2</v>
       </c>
-      <c r="E42">
-        <v>27.039000000000001</v>
+      <c r="E42" t="s">
+        <v>22</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
       </c>
-      <c r="G42">
-        <v>27.039000000000001</v>
+      <c r="G42" t="s">
+        <v>16</v>
       </c>
       <c r="H42" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -1962,7 +2038,374 @@
         <v>18</v>
       </c>
     </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>60</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" t="s">
+        <v>53</v>
+      </c>
+      <c r="F50" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>75</v>
+      </c>
+      <c r="H50" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>64</v>
+      </c>
+      <c r="B51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51">
+        <v>13</v>
+      </c>
+      <c r="F51" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" t="s">
+        <v>77</v>
+      </c>
+      <c r="H51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>65</v>
+      </c>
+      <c r="B52" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52">
+        <v>13</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>66</v>
+      </c>
+      <c r="B53" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" t="s">
+        <v>94</v>
+      </c>
+      <c r="E53" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" t="s">
+        <v>82</v>
+      </c>
+      <c r="G53" t="s">
+        <v>83</v>
+      </c>
+      <c r="H53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54" t="s">
+        <v>82</v>
+      </c>
+      <c r="G54" t="s">
+        <v>85</v>
+      </c>
+      <c r="H54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>36</v>
+      </c>
+      <c r="B55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" t="s">
+        <v>82</v>
+      </c>
+      <c r="G55" t="s">
+        <v>86</v>
+      </c>
+      <c r="H55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>37</v>
+      </c>
+      <c r="B56" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F56" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>50</v>
+      </c>
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57" t="s">
+        <v>81</v>
+      </c>
+      <c r="F57" t="s">
+        <v>82</v>
+      </c>
+      <c r="G57" t="s">
+        <v>89</v>
+      </c>
+      <c r="H57" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>49</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" t="s">
+        <v>80</v>
+      </c>
+      <c r="D58" t="s">
+        <v>88</v>
+      </c>
+      <c r="E58" t="s">
+        <v>81</v>
+      </c>
+      <c r="F58" t="s">
+        <v>82</v>
+      </c>
+      <c r="G58" t="s">
+        <v>87</v>
+      </c>
+      <c r="H58" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>47</v>
+      </c>
+      <c r="B59" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E59" t="s">
+        <v>81</v>
+      </c>
+      <c r="F59" t="s">
+        <v>82</v>
+      </c>
+      <c r="G59" t="s">
+        <v>91</v>
+      </c>
+      <c r="H59" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>30</v>
+      </c>
+      <c r="B60" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60" t="s">
+        <v>90</v>
+      </c>
+      <c r="E60" t="s">
+        <v>81</v>
+      </c>
+      <c r="F60" t="s">
+        <v>82</v>
+      </c>
+      <c r="G60" t="s">
+        <v>92</v>
+      </c>
+      <c r="H60" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>75</v>
+      </c>
+      <c r="B61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" t="s">
+        <v>93</v>
+      </c>
+      <c r="E61" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61" t="s">
+        <v>82</v>
+      </c>
+      <c r="G61" t="s">
+        <v>95</v>
+      </c>
+      <c r="H61" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>76</v>
+      </c>
+      <c r="B62" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" t="s">
+        <v>80</v>
+      </c>
+      <c r="D62" t="s">
+        <v>93</v>
+      </c>
+      <c r="E62" t="s">
+        <v>81</v>
+      </c>
+      <c r="F62" t="s">
+        <v>82</v>
+      </c>
+      <c r="G62" t="s">
+        <v>96</v>
+      </c>
+      <c r="H62" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q48">
+    <sortCondition ref="A2:A48"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>